<commit_message>
feat: magic stone loot
</commit_message>
<xml_diff>
--- a/Assets/Scripts/EditorTool/Terasurware/MagicStones.xlsx
+++ b/Assets/Scripts/EditorTool/Terasurware/MagicStones.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="MagicStones" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -129,12 +129,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -335,3375 +339,3375 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>4101111</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>4101112</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>4101113</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>4101121</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>4101122</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>4101123</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>4102111</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>4102112</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>4102113</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>4102121</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>4102122</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>4102123</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>4103111</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>4103112</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>4103113</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <v>4103121</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>4103122</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>4103123</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>4104111</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <v>4104112</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <v>4104113</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <v>4104121</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>4104122</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>4104123</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>4105111</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <v>4105112</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <v>4105113</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>4105121</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="2" t="n">
         <v>4105122</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <v>4105123</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <v>4106111</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <v>4106112</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <v>4106113</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>4106121</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="2" t="n">
         <v>4106122</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="2" t="n">
         <v>4106123</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="2" t="n">
         <v>4107111</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <v>4107112</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>4107113</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>4107121</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <v>4107122</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="2" t="n">
         <v>4107123</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>4108111</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="2" t="n">
         <v>4108112</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="2" t="n">
         <v>4108113</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>4108121</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="2" t="n">
         <v>4108122</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="2" t="n">
         <v>4108123</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="2" t="n">
         <v>4109111</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="2" t="n">
         <v>4109112</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="2" t="n">
         <v>4109113</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="2" t="n">
         <v>4109121</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="2" t="n">
         <v>4109122</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="2" t="n">
         <v>4109123</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="2" t="n">
         <v>4110111</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="2" t="n">
         <v>4110112</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="2" t="n">
         <v>4110113</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="2" t="n">
         <v>4110121</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="2" t="n">
         <v>4110122</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="2" t="n">
         <v>4110123</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="2" t="n">
         <v>4201111</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="2" t="n">
         <v>4201112</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="2" t="n">
         <v>4201113</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="2" t="n">
         <v>4201121</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="2" t="n">
         <v>4201122</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="2" t="n">
         <v>4201123</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="2" t="n">
         <v>4202111</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="2" t="n">
         <v>4202112</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="2" t="n">
         <v>4202113</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="2" t="n">
         <v>4202121</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="2" t="n">
         <v>4202122</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="2" t="n">
         <v>4202123</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="2" t="n">
         <v>4203111</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="2" t="n">
         <v>4203112</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="2" t="n">
         <v>4203113</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="2" t="n">
         <v>4203121</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="2" t="n">
         <v>4203122</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="2" t="n">
         <v>4203123</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="2" t="n">
         <v>4204111</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="2" t="n">
         <v>4204112</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="2" t="n">
         <v>4204113</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="2" t="n">
         <v>4204121</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="2" t="n">
         <v>4204122</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="2" t="n">
         <v>4204123</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="2" t="n">
         <v>4205111</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="2" t="n">
         <v>4205112</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="2" t="n">
         <v>4205113</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="2" t="n">
         <v>4205121</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="2" t="n">
         <v>4205122</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="2" t="n">
         <v>4205123</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="2" t="n">
         <v>4206111</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="2" t="n">
         <v>4206112</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="2" t="n">
         <v>4206113</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="2" t="n">
         <v>4206121</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="2" t="n">
         <v>4206122</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="2" t="n">
         <v>4206123</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="2" t="n">
         <v>4207111</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="2" t="n">
         <v>4207112</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="2" t="n">
         <v>4207113</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="2" t="n">
         <v>4207121</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="2" t="n">
         <v>4207122</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="2" t="n">
         <v>4207123</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="2" t="n">
         <v>4208111</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="2" t="n">
         <v>4208112</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="2" t="n">
         <v>4208113</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="2" t="n">
         <v>4208121</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="2" t="n">
         <v>4208122</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="2" t="n">
         <v>4208123</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="2" t="n">
         <v>4209111</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="2" t="n">
         <v>4209112</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="2" t="n">
         <v>4209113</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="2" t="n">
         <v>4209121</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="2" t="n">
         <v>4209122</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="2" t="n">
         <v>4209123</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="2" t="n">
         <v>4210111</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="2" t="n">
         <v>4210112</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="2" t="n">
         <v>4210113</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="2" t="n">
         <v>4210121</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="2" t="n">
         <v>4210122</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="2" t="n">
         <v>4210123</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="2" t="n">
         <v>4301111</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="2" t="n">
         <v>4301112</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="2" t="n">
         <v>4301113</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="2" t="n">
         <v>4301121</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="2" t="n">
         <v>4301122</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="2" t="n">
         <v>4301123</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="2" t="n">
         <v>4302111</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="2" t="n">
         <v>4302112</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="2" t="n">
         <v>4302113</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="2" t="n">
         <v>4302121</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="2" t="n">
         <v>4302122</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="2" t="n">
         <v>4302123</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="2" t="n">
         <v>4303111</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="2" t="n">
         <v>4303112</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="2" t="n">
         <v>4303113</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="2" t="n">
         <v>4303121</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="2" t="n">
         <v>4303122</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="2" t="n">
         <v>4303123</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="2" t="n">
         <v>4304111</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="2" t="n">
         <v>4304112</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="2" t="n">
         <v>4304113</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="2" t="n">
         <v>4304121</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="2" t="n">
         <v>4304122</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="2" t="n">
         <v>4304123</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="2" t="n">
         <v>4305111</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="2" t="n">
         <v>4305112</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="2" t="n">
         <v>4305113</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="2" t="n">
         <v>4305121</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="2" t="n">
         <v>4305122</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="2" t="n">
         <v>4305123</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="2" t="n">
         <v>4306111</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="2" t="n">
         <v>4306112</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="n">
+      <c r="A154" s="2" t="n">
         <v>4306113</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="n">
+      <c r="A155" s="2" t="n">
         <v>4306121</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
+      <c r="A156" s="2" t="n">
         <v>4306122</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="n">
+      <c r="A157" s="2" t="n">
         <v>4306123</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B157" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="n">
+      <c r="A158" s="2" t="n">
         <v>4307111</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="n">
+      <c r="A159" s="2" t="n">
         <v>4307112</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
+      <c r="A160" s="2" t="n">
         <v>4307113</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
+      <c r="A161" s="2" t="n">
         <v>4307121</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="n">
+      <c r="A162" s="2" t="n">
         <v>4307122</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="n">
+      <c r="A163" s="2" t="n">
         <v>4307123</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="n">
+      <c r="A164" s="2" t="n">
         <v>4308111</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="n">
+      <c r="A165" s="2" t="n">
         <v>4308112</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="n">
+      <c r="A166" s="2" t="n">
         <v>4308113</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="n">
+      <c r="A167" s="2" t="n">
         <v>4308121</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="n">
+      <c r="A168" s="2" t="n">
         <v>4308122</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="n">
+      <c r="A169" s="2" t="n">
         <v>4308123</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="n">
+      <c r="A170" s="2" t="n">
         <v>4309111</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B170" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="n">
+      <c r="A171" s="2" t="n">
         <v>4309112</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B171" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="n">
+      <c r="A172" s="2" t="n">
         <v>4309113</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B172" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="n">
+      <c r="A173" s="2" t="n">
         <v>4309121</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B173" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="n">
+      <c r="A174" s="2" t="n">
         <v>4309122</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B174" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="n">
+      <c r="A175" s="2" t="n">
         <v>4309123</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B175" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="n">
+      <c r="A176" s="2" t="n">
         <v>4310111</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="n">
+      <c r="A177" s="2" t="n">
         <v>4310112</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B177" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="n">
+      <c r="A178" s="2" t="n">
         <v>4310113</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B178" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="n">
+      <c r="A179" s="2" t="n">
         <v>4310121</v>
       </c>
-      <c r="B179" s="1" t="s">
+      <c r="B179" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="n">
+      <c r="A180" s="2" t="n">
         <v>4310122</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B180" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="n">
+      <c r="A181" s="2" t="n">
         <v>4310123</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B181" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="n">
+      <c r="A182" s="2" t="n">
         <v>4401111</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="B182" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="n">
+      <c r="A183" s="2" t="n">
         <v>4401112</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B183" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="n">
+      <c r="A184" s="2" t="n">
         <v>4401113</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B184" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="n">
+      <c r="A185" s="2" t="n">
         <v>4401121</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="1" t="n">
+      <c r="A186" s="2" t="n">
         <v>4401122</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="B186" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="n">
+      <c r="A187" s="2" t="n">
         <v>4401123</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="B187" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="n">
+      <c r="A188" s="2" t="n">
         <v>4402111</v>
       </c>
-      <c r="B188" s="1" t="s">
+      <c r="B188" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="1" t="n">
+      <c r="A189" s="2" t="n">
         <v>4402112</v>
       </c>
-      <c r="B189" s="1" t="s">
+      <c r="B189" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="n">
+      <c r="A190" s="2" t="n">
         <v>4402113</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="B190" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="1" t="n">
+      <c r="A191" s="2" t="n">
         <v>4402121</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B191" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="1" t="n">
+      <c r="A192" s="2" t="n">
         <v>4402122</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B192" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="1" t="n">
+      <c r="A193" s="2" t="n">
         <v>4402123</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="B193" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="1" t="n">
+      <c r="A194" s="2" t="n">
         <v>4403111</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="B194" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="1" t="n">
+      <c r="A195" s="2" t="n">
         <v>4403112</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="B195" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="1" t="n">
+      <c r="A196" s="2" t="n">
         <v>4403113</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="B196" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="1" t="n">
+      <c r="A197" s="2" t="n">
         <v>4403121</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="B197" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="n">
+      <c r="A198" s="2" t="n">
         <v>4403122</v>
       </c>
-      <c r="B198" s="1" t="s">
+      <c r="B198" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="1" t="n">
+      <c r="A199" s="2" t="n">
         <v>4403123</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B199" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="n">
+      <c r="A200" s="2" t="n">
         <v>4404111</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B200" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="1" t="n">
+      <c r="A201" s="2" t="n">
         <v>4404112</v>
       </c>
-      <c r="B201" s="1" t="s">
+      <c r="B201" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="n">
+      <c r="A202" s="2" t="n">
         <v>4404113</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B202" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="n">
+      <c r="A203" s="2" t="n">
         <v>4404121</v>
       </c>
-      <c r="B203" s="1" t="s">
+      <c r="B203" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="1" t="n">
+      <c r="A204" s="2" t="n">
         <v>4404122</v>
       </c>
-      <c r="B204" s="1" t="s">
+      <c r="B204" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="1" t="n">
+      <c r="A205" s="2" t="n">
         <v>4404123</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B205" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="1" t="n">
+      <c r="A206" s="2" t="n">
         <v>4405111</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="B206" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1" t="n">
+      <c r="A207" s="2" t="n">
         <v>4405112</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B207" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1" t="n">
+      <c r="A208" s="2" t="n">
         <v>4405113</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B208" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="1" t="n">
+      <c r="A209" s="2" t="n">
         <v>4405121</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="B209" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="1" t="n">
+      <c r="A210" s="2" t="n">
         <v>4405122</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="B210" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="1" t="n">
+      <c r="A211" s="2" t="n">
         <v>4405123</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="B211" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="1" t="n">
+      <c r="A212" s="2" t="n">
         <v>4406111</v>
       </c>
-      <c r="B212" s="1" t="s">
+      <c r="B212" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="1" t="n">
+      <c r="A213" s="2" t="n">
         <v>4406112</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="B213" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="1" t="n">
+      <c r="A214" s="2" t="n">
         <v>4406113</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="B214" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="1" t="n">
+      <c r="A215" s="2" t="n">
         <v>4406121</v>
       </c>
-      <c r="B215" s="1" t="s">
+      <c r="B215" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="n">
+      <c r="A216" s="2" t="n">
         <v>4406122</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B216" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="1" t="n">
+      <c r="A217" s="2" t="n">
         <v>4406123</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B217" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="1" t="n">
+      <c r="A218" s="2" t="n">
         <v>4407111</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="B218" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1" t="n">
+      <c r="A219" s="2" t="n">
         <v>4407112</v>
       </c>
-      <c r="B219" s="1" t="s">
+      <c r="B219" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="1" t="n">
+      <c r="A220" s="2" t="n">
         <v>4407113</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B220" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="1" t="n">
+      <c r="A221" s="2" t="n">
         <v>4407121</v>
       </c>
-      <c r="B221" s="1" t="s">
+      <c r="B221" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="1" t="n">
+      <c r="A222" s="2" t="n">
         <v>4407122</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B222" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="1" t="n">
+      <c r="A223" s="2" t="n">
         <v>4407123</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B223" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="1" t="n">
+      <c r="A224" s="2" t="n">
         <v>4408111</v>
       </c>
-      <c r="B224" s="1" t="s">
+      <c r="B224" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="1" t="n">
+      <c r="A225" s="2" t="n">
         <v>4408112</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B225" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="1" t="n">
+      <c r="A226" s="2" t="n">
         <v>4408113</v>
       </c>
-      <c r="B226" s="1" t="s">
+      <c r="B226" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="1" t="n">
+      <c r="A227" s="2" t="n">
         <v>4408121</v>
       </c>
-      <c r="B227" s="1" t="s">
+      <c r="B227" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="1" t="n">
+      <c r="A228" s="2" t="n">
         <v>4408122</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B228" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="1" t="n">
+      <c r="A229" s="2" t="n">
         <v>4408123</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B229" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="1" t="n">
+      <c r="A230" s="2" t="n">
         <v>4409111</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B230" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="1" t="n">
+      <c r="A231" s="2" t="n">
         <v>4409112</v>
       </c>
-      <c r="B231" s="1" t="s">
+      <c r="B231" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="1" t="n">
+      <c r="A232" s="2" t="n">
         <v>4409113</v>
       </c>
-      <c r="B232" s="1" t="s">
+      <c r="B232" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="1" t="n">
+      <c r="A233" s="2" t="n">
         <v>4409121</v>
       </c>
-      <c r="B233" s="1" t="s">
+      <c r="B233" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="1" t="n">
+      <c r="A234" s="2" t="n">
         <v>4409122</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="B234" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="1" t="n">
+      <c r="A235" s="2" t="n">
         <v>4409123</v>
       </c>
-      <c r="B235" s="1" t="s">
+      <c r="B235" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="1" t="n">
+      <c r="A236" s="2" t="n">
         <v>4410111</v>
       </c>
-      <c r="B236" s="1" t="s">
+      <c r="B236" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="1" t="n">
+      <c r="A237" s="2" t="n">
         <v>4410112</v>
       </c>
-      <c r="B237" s="1" t="s">
+      <c r="B237" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="1" t="n">
+      <c r="A238" s="2" t="n">
         <v>4410113</v>
       </c>
-      <c r="B238" s="1" t="s">
+      <c r="B238" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="1" t="n">
+      <c r="A239" s="2" t="n">
         <v>4410121</v>
       </c>
-      <c r="B239" s="1" t="s">
+      <c r="B239" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="1" t="n">
+      <c r="A240" s="2" t="n">
         <v>4410122</v>
       </c>
-      <c r="B240" s="1" t="s">
+      <c r="B240" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="1" t="n">
+      <c r="A241" s="2" t="n">
         <v>4410123</v>
       </c>
-      <c r="B241" s="1" t="s">
+      <c r="B241" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="1" t="n">
+      <c r="A242" s="2" t="n">
         <v>4501111</v>
       </c>
-      <c r="B242" s="1" t="s">
+      <c r="B242" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="1" t="n">
+      <c r="A243" s="2" t="n">
         <v>4501112</v>
       </c>
-      <c r="B243" s="1" t="s">
+      <c r="B243" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="1" t="n">
+      <c r="A244" s="2" t="n">
         <v>4501113</v>
       </c>
-      <c r="B244" s="1" t="s">
+      <c r="B244" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="1" t="n">
+      <c r="A245" s="2" t="n">
         <v>4501121</v>
       </c>
-      <c r="B245" s="1" t="s">
+      <c r="B245" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="1" t="n">
+      <c r="A246" s="2" t="n">
         <v>4501122</v>
       </c>
-      <c r="B246" s="1" t="s">
+      <c r="B246" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="1" t="n">
+      <c r="A247" s="2" t="n">
         <v>4501123</v>
       </c>
-      <c r="B247" s="1" t="s">
+      <c r="B247" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="1" t="n">
+      <c r="A248" s="2" t="n">
         <v>4502111</v>
       </c>
-      <c r="B248" s="1" t="s">
+      <c r="B248" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="1" t="n">
+      <c r="A249" s="2" t="n">
         <v>4502112</v>
       </c>
-      <c r="B249" s="1" t="s">
+      <c r="B249" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="1" t="n">
+      <c r="A250" s="2" t="n">
         <v>4502113</v>
       </c>
-      <c r="B250" s="1" t="s">
+      <c r="B250" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="1" t="n">
+      <c r="A251" s="2" t="n">
         <v>4502121</v>
       </c>
-      <c r="B251" s="1" t="s">
+      <c r="B251" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="1" t="n">
+      <c r="A252" s="2" t="n">
         <v>4502122</v>
       </c>
-      <c r="B252" s="1" t="s">
+      <c r="B252" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="1" t="n">
+      <c r="A253" s="2" t="n">
         <v>4502123</v>
       </c>
-      <c r="B253" s="1" t="s">
+      <c r="B253" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="1" t="n">
+      <c r="A254" s="2" t="n">
         <v>4503111</v>
       </c>
-      <c r="B254" s="1" t="s">
+      <c r="B254" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="1" t="n">
+      <c r="A255" s="2" t="n">
         <v>4503112</v>
       </c>
-      <c r="B255" s="1" t="s">
+      <c r="B255" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="1" t="n">
+      <c r="A256" s="2" t="n">
         <v>4503113</v>
       </c>
-      <c r="B256" s="1" t="s">
+      <c r="B256" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="1" t="n">
+      <c r="A257" s="2" t="n">
         <v>4503121</v>
       </c>
-      <c r="B257" s="1" t="s">
+      <c r="B257" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="1" t="n">
+      <c r="A258" s="2" t="n">
         <v>4503122</v>
       </c>
-      <c r="B258" s="1" t="s">
+      <c r="B258" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="1" t="n">
+      <c r="A259" s="2" t="n">
         <v>4503123</v>
       </c>
-      <c r="B259" s="1" t="s">
+      <c r="B259" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="1" t="n">
+      <c r="A260" s="2" t="n">
         <v>4504111</v>
       </c>
-      <c r="B260" s="1" t="s">
+      <c r="B260" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="1" t="n">
+      <c r="A261" s="2" t="n">
         <v>4504112</v>
       </c>
-      <c r="B261" s="1" t="s">
+      <c r="B261" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="1" t="n">
+      <c r="A262" s="2" t="n">
         <v>4504113</v>
       </c>
-      <c r="B262" s="1" t="s">
+      <c r="B262" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="1" t="n">
+      <c r="A263" s="2" t="n">
         <v>4504121</v>
       </c>
-      <c r="B263" s="1" t="s">
+      <c r="B263" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="1" t="n">
+      <c r="A264" s="2" t="n">
         <v>4504122</v>
       </c>
-      <c r="B264" s="1" t="s">
+      <c r="B264" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="1" t="n">
+      <c r="A265" s="2" t="n">
         <v>4504123</v>
       </c>
-      <c r="B265" s="1" t="s">
+      <c r="B265" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="1" t="n">
+      <c r="A266" s="2" t="n">
         <v>4505111</v>
       </c>
-      <c r="B266" s="1" t="s">
+      <c r="B266" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="1" t="n">
+      <c r="A267" s="2" t="n">
         <v>4505112</v>
       </c>
-      <c r="B267" s="1" t="s">
+      <c r="B267" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="1" t="n">
+      <c r="A268" s="2" t="n">
         <v>4505113</v>
       </c>
-      <c r="B268" s="1" t="s">
+      <c r="B268" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="1" t="n">
+      <c r="A269" s="2" t="n">
         <v>4505121</v>
       </c>
-      <c r="B269" s="1" t="s">
+      <c r="B269" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="1" t="n">
+      <c r="A270" s="2" t="n">
         <v>4505122</v>
       </c>
-      <c r="B270" s="1" t="s">
+      <c r="B270" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="1" t="n">
+      <c r="A271" s="2" t="n">
         <v>4505123</v>
       </c>
-      <c r="B271" s="1" t="s">
+      <c r="B271" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="1" t="n">
+      <c r="A272" s="2" t="n">
         <v>4506111</v>
       </c>
-      <c r="B272" s="1" t="s">
+      <c r="B272" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="1" t="n">
+      <c r="A273" s="2" t="n">
         <v>4506112</v>
       </c>
-      <c r="B273" s="1" t="s">
+      <c r="B273" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1" t="n">
+      <c r="A274" s="2" t="n">
         <v>4506113</v>
       </c>
-      <c r="B274" s="1" t="s">
+      <c r="B274" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="1" t="n">
+      <c r="A275" s="2" t="n">
         <v>4506121</v>
       </c>
-      <c r="B275" s="1" t="s">
+      <c r="B275" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="1" t="n">
+      <c r="A276" s="2" t="n">
         <v>4506122</v>
       </c>
-      <c r="B276" s="1" t="s">
+      <c r="B276" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="1" t="n">
+      <c r="A277" s="2" t="n">
         <v>4506123</v>
       </c>
-      <c r="B277" s="1" t="s">
+      <c r="B277" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="1" t="n">
+      <c r="A278" s="2" t="n">
         <v>4507111</v>
       </c>
-      <c r="B278" s="1" t="s">
+      <c r="B278" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="1" t="n">
+      <c r="A279" s="2" t="n">
         <v>4507112</v>
       </c>
-      <c r="B279" s="1" t="s">
+      <c r="B279" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="1" t="n">
+      <c r="A280" s="2" t="n">
         <v>4507113</v>
       </c>
-      <c r="B280" s="1" t="s">
+      <c r="B280" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="1" t="n">
+      <c r="A281" s="2" t="n">
         <v>4507121</v>
       </c>
-      <c r="B281" s="1" t="s">
+      <c r="B281" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="1" t="n">
+      <c r="A282" s="2" t="n">
         <v>4507122</v>
       </c>
-      <c r="B282" s="1" t="s">
+      <c r="B282" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="1" t="n">
+      <c r="A283" s="2" t="n">
         <v>4507123</v>
       </c>
-      <c r="B283" s="1" t="s">
+      <c r="B283" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="1" t="n">
+      <c r="A284" s="2" t="n">
         <v>4508111</v>
       </c>
-      <c r="B284" s="1" t="s">
+      <c r="B284" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="1" t="n">
+      <c r="A285" s="2" t="n">
         <v>4508112</v>
       </c>
-      <c r="B285" s="1" t="s">
+      <c r="B285" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="1" t="n">
+      <c r="A286" s="2" t="n">
         <v>4508113</v>
       </c>
-      <c r="B286" s="1" t="s">
+      <c r="B286" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="1" t="n">
+      <c r="A287" s="2" t="n">
         <v>4508121</v>
       </c>
-      <c r="B287" s="1" t="s">
+      <c r="B287" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="1" t="n">
+      <c r="A288" s="2" t="n">
         <v>4508122</v>
       </c>
-      <c r="B288" s="1" t="s">
+      <c r="B288" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="1" t="n">
+      <c r="A289" s="2" t="n">
         <v>4508123</v>
       </c>
-      <c r="B289" s="1" t="s">
+      <c r="B289" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="1" t="n">
+      <c r="A290" s="2" t="n">
         <v>4509111</v>
       </c>
-      <c r="B290" s="1" t="s">
+      <c r="B290" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="1" t="n">
+      <c r="A291" s="2" t="n">
         <v>4509112</v>
       </c>
-      <c r="B291" s="1" t="s">
+      <c r="B291" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="1" t="n">
+      <c r="A292" s="2" t="n">
         <v>4509113</v>
       </c>
-      <c r="B292" s="1" t="s">
+      <c r="B292" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="1" t="n">
+      <c r="A293" s="2" t="n">
         <v>4509121</v>
       </c>
-      <c r="B293" s="1" t="s">
+      <c r="B293" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="1" t="n">
+      <c r="A294" s="2" t="n">
         <v>4509122</v>
       </c>
-      <c r="B294" s="1" t="s">
+      <c r="B294" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="1" t="n">
+      <c r="A295" s="2" t="n">
         <v>4509123</v>
       </c>
-      <c r="B295" s="1" t="s">
+      <c r="B295" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="1" t="n">
+      <c r="A296" s="2" t="n">
         <v>4510111</v>
       </c>
-      <c r="B296" s="1" t="s">
+      <c r="B296" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="1" t="n">
+      <c r="A297" s="2" t="n">
         <v>4510112</v>
       </c>
-      <c r="B297" s="1" t="s">
+      <c r="B297" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="1" t="n">
+      <c r="A298" s="2" t="n">
         <v>4510113</v>
       </c>
-      <c r="B298" s="1" t="s">
+      <c r="B298" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="1" t="n">
+      <c r="A299" s="2" t="n">
         <v>4510121</v>
       </c>
-      <c r="B299" s="1" t="s">
+      <c r="B299" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="1" t="n">
+      <c r="A300" s="2" t="n">
         <v>4510122</v>
       </c>
-      <c r="B300" s="1" t="s">
+      <c r="B300" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="1" t="n">
+      <c r="A301" s="2" t="n">
         <v>4510123</v>
       </c>
-      <c r="B301" s="1" t="s">
+      <c r="B301" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="1" t="n">
+      <c r="A302" s="2" t="n">
         <v>4601111</v>
       </c>
-      <c r="B302" s="1" t="s">
+      <c r="B302" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="1" t="n">
+      <c r="A303" s="2" t="n">
         <v>4601112</v>
       </c>
-      <c r="B303" s="1" t="s">
+      <c r="B303" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="1" t="n">
+      <c r="A304" s="2" t="n">
         <v>4601113</v>
       </c>
-      <c r="B304" s="1" t="s">
+      <c r="B304" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="1" t="n">
+      <c r="A305" s="2" t="n">
         <v>4601121</v>
       </c>
-      <c r="B305" s="1" t="s">
+      <c r="B305" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="1" t="n">
+      <c r="A306" s="2" t="n">
         <v>4601122</v>
       </c>
-      <c r="B306" s="1" t="s">
+      <c r="B306" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="1" t="n">
+      <c r="A307" s="2" t="n">
         <v>4601123</v>
       </c>
-      <c r="B307" s="1" t="s">
+      <c r="B307" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="1" t="n">
+      <c r="A308" s="2" t="n">
         <v>4602111</v>
       </c>
-      <c r="B308" s="1" t="s">
+      <c r="B308" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="1" t="n">
+      <c r="A309" s="2" t="n">
         <v>4602112</v>
       </c>
-      <c r="B309" s="1" t="s">
+      <c r="B309" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="1" t="n">
+      <c r="A310" s="2" t="n">
         <v>4602113</v>
       </c>
-      <c r="B310" s="1" t="s">
+      <c r="B310" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="1" t="n">
+      <c r="A311" s="2" t="n">
         <v>4602121</v>
       </c>
-      <c r="B311" s="1" t="s">
+      <c r="B311" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="1" t="n">
+      <c r="A312" s="2" t="n">
         <v>4602122</v>
       </c>
-      <c r="B312" s="1" t="s">
+      <c r="B312" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="1" t="n">
+      <c r="A313" s="2" t="n">
         <v>4602123</v>
       </c>
-      <c r="B313" s="1" t="s">
+      <c r="B313" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="1" t="n">
+      <c r="A314" s="2" t="n">
         <v>4603111</v>
       </c>
-      <c r="B314" s="1" t="s">
+      <c r="B314" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="1" t="n">
+      <c r="A315" s="2" t="n">
         <v>4603112</v>
       </c>
-      <c r="B315" s="1" t="s">
+      <c r="B315" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="1" t="n">
+      <c r="A316" s="2" t="n">
         <v>4603113</v>
       </c>
-      <c r="B316" s="1" t="s">
+      <c r="B316" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="1" t="n">
+      <c r="A317" s="2" t="n">
         <v>4603121</v>
       </c>
-      <c r="B317" s="1" t="s">
+      <c r="B317" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="1" t="n">
+      <c r="A318" s="2" t="n">
         <v>4603122</v>
       </c>
-      <c r="B318" s="1" t="s">
+      <c r="B318" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="1" t="n">
+      <c r="A319" s="2" t="n">
         <v>4603123</v>
       </c>
-      <c r="B319" s="1" t="s">
+      <c r="B319" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="1" t="n">
+      <c r="A320" s="2" t="n">
         <v>4604111</v>
       </c>
-      <c r="B320" s="1" t="s">
+      <c r="B320" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="1" t="n">
+      <c r="A321" s="2" t="n">
         <v>4604112</v>
       </c>
-      <c r="B321" s="1" t="s">
+      <c r="B321" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="1" t="n">
+      <c r="A322" s="2" t="n">
         <v>4604113</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="B322" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="1" t="n">
+      <c r="A323" s="2" t="n">
         <v>4604121</v>
       </c>
-      <c r="B323" s="1" t="s">
+      <c r="B323" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="1" t="n">
+      <c r="A324" s="2" t="n">
         <v>4604122</v>
       </c>
-      <c r="B324" s="1" t="s">
+      <c r="B324" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="1" t="n">
+      <c r="A325" s="2" t="n">
         <v>4604123</v>
       </c>
-      <c r="B325" s="1" t="s">
+      <c r="B325" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="1" t="n">
+      <c r="A326" s="2" t="n">
         <v>4605111</v>
       </c>
-      <c r="B326" s="1" t="s">
+      <c r="B326" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="1" t="n">
+      <c r="A327" s="2" t="n">
         <v>4605112</v>
       </c>
-      <c r="B327" s="1" t="s">
+      <c r="B327" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="1" t="n">
+      <c r="A328" s="2" t="n">
         <v>4605113</v>
       </c>
-      <c r="B328" s="1" t="s">
+      <c r="B328" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="1" t="n">
+      <c r="A329" s="2" t="n">
         <v>4605121</v>
       </c>
-      <c r="B329" s="1" t="s">
+      <c r="B329" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="1" t="n">
+      <c r="A330" s="2" t="n">
         <v>4605122</v>
       </c>
-      <c r="B330" s="1" t="s">
+      <c r="B330" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="1" t="n">
+      <c r="A331" s="2" t="n">
         <v>4605123</v>
       </c>
-      <c r="B331" s="1" t="s">
+      <c r="B331" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="1" t="n">
+      <c r="A332" s="2" t="n">
         <v>4606111</v>
       </c>
-      <c r="B332" s="1" t="s">
+      <c r="B332" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="1" t="n">
+      <c r="A333" s="2" t="n">
         <v>4606112</v>
       </c>
-      <c r="B333" s="1" t="s">
+      <c r="B333" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="1" t="n">
+      <c r="A334" s="2" t="n">
         <v>4606113</v>
       </c>
-      <c r="B334" s="1" t="s">
+      <c r="B334" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="1" t="n">
+      <c r="A335" s="2" t="n">
         <v>4606121</v>
       </c>
-      <c r="B335" s="1" t="s">
+      <c r="B335" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="1" t="n">
+      <c r="A336" s="2" t="n">
         <v>4606122</v>
       </c>
-      <c r="B336" s="1" t="s">
+      <c r="B336" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="1" t="n">
+      <c r="A337" s="2" t="n">
         <v>4606123</v>
       </c>
-      <c r="B337" s="1" t="s">
+      <c r="B337" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="1" t="n">
+      <c r="A338" s="2" t="n">
         <v>4607111</v>
       </c>
-      <c r="B338" s="1" t="s">
+      <c r="B338" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="1" t="n">
+      <c r="A339" s="2" t="n">
         <v>4607112</v>
       </c>
-      <c r="B339" s="1" t="s">
+      <c r="B339" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="1" t="n">
+      <c r="A340" s="2" t="n">
         <v>4607113</v>
       </c>
-      <c r="B340" s="1" t="s">
+      <c r="B340" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="1" t="n">
+      <c r="A341" s="2" t="n">
         <v>4607121</v>
       </c>
-      <c r="B341" s="1" t="s">
+      <c r="B341" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="1" t="n">
+      <c r="A342" s="2" t="n">
         <v>4607122</v>
       </c>
-      <c r="B342" s="1" t="s">
+      <c r="B342" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="1" t="n">
+      <c r="A343" s="2" t="n">
         <v>4607123</v>
       </c>
-      <c r="B343" s="1" t="s">
+      <c r="B343" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="1" t="n">
+      <c r="A344" s="2" t="n">
         <v>4608111</v>
       </c>
-      <c r="B344" s="1" t="s">
+      <c r="B344" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="1" t="n">
+      <c r="A345" s="2" t="n">
         <v>4608112</v>
       </c>
-      <c r="B345" s="1" t="s">
+      <c r="B345" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="1" t="n">
+      <c r="A346" s="2" t="n">
         <v>4608113</v>
       </c>
-      <c r="B346" s="1" t="s">
+      <c r="B346" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="1" t="n">
+      <c r="A347" s="2" t="n">
         <v>4608121</v>
       </c>
-      <c r="B347" s="1" t="s">
+      <c r="B347" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="1" t="n">
+      <c r="A348" s="2" t="n">
         <v>4608122</v>
       </c>
-      <c r="B348" s="1" t="s">
+      <c r="B348" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="1" t="n">
+      <c r="A349" s="2" t="n">
         <v>4608123</v>
       </c>
-      <c r="B349" s="1" t="s">
+      <c r="B349" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="1" t="n">
+      <c r="A350" s="2" t="n">
         <v>4609111</v>
       </c>
-      <c r="B350" s="1" t="s">
+      <c r="B350" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="1" t="n">
+      <c r="A351" s="2" t="n">
         <v>4609112</v>
       </c>
-      <c r="B351" s="1" t="s">
+      <c r="B351" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="1" t="n">
+      <c r="A352" s="2" t="n">
         <v>4609113</v>
       </c>
-      <c r="B352" s="1" t="s">
+      <c r="B352" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="1" t="n">
+      <c r="A353" s="2" t="n">
         <v>4609121</v>
       </c>
-      <c r="B353" s="1" t="s">
+      <c r="B353" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="1" t="n">
+      <c r="A354" s="2" t="n">
         <v>4609122</v>
       </c>
-      <c r="B354" s="1" t="s">
+      <c r="B354" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="1" t="n">
+      <c r="A355" s="2" t="n">
         <v>4609123</v>
       </c>
-      <c r="B355" s="1" t="s">
+      <c r="B355" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="1" t="n">
+      <c r="A356" s="2" t="n">
         <v>4610111</v>
       </c>
-      <c r="B356" s="1" t="s">
+      <c r="B356" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="1" t="n">
+      <c r="A357" s="2" t="n">
         <v>4610112</v>
       </c>
-      <c r="B357" s="1" t="s">
+      <c r="B357" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="1" t="n">
+      <c r="A358" s="2" t="n">
         <v>4610113</v>
       </c>
-      <c r="B358" s="1" t="s">
+      <c r="B358" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="1" t="n">
+      <c r="A359" s="2" t="n">
         <v>4610121</v>
       </c>
-      <c r="B359" s="1" t="s">
+      <c r="B359" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="1" t="n">
+      <c r="A360" s="2" t="n">
         <v>4610122</v>
       </c>
-      <c r="B360" s="1" t="s">
+      <c r="B360" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="1" t="n">
+      <c r="A361" s="2" t="n">
         <v>4610123</v>
       </c>
-      <c r="B361" s="1" t="s">
+      <c r="B361" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="1" t="n">
+      <c r="A362" s="2" t="n">
         <v>4701111</v>
       </c>
-      <c r="B362" s="1" t="s">
+      <c r="B362" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="1" t="n">
+      <c r="A363" s="2" t="n">
         <v>4701112</v>
       </c>
-      <c r="B363" s="1" t="s">
+      <c r="B363" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="1" t="n">
+      <c r="A364" s="2" t="n">
         <v>4701113</v>
       </c>
-      <c r="B364" s="1" t="s">
+      <c r="B364" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="1" t="n">
+      <c r="A365" s="2" t="n">
         <v>4701121</v>
       </c>
-      <c r="B365" s="1" t="s">
+      <c r="B365" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="1" t="n">
+      <c r="A366" s="2" t="n">
         <v>4701122</v>
       </c>
-      <c r="B366" s="1" t="s">
+      <c r="B366" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="1" t="n">
+      <c r="A367" s="2" t="n">
         <v>4701123</v>
       </c>
-      <c r="B367" s="1" t="s">
+      <c r="B367" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="1" t="n">
+      <c r="A368" s="2" t="n">
         <v>4702111</v>
       </c>
-      <c r="B368" s="1" t="s">
+      <c r="B368" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="1" t="n">
+      <c r="A369" s="2" t="n">
         <v>4702112</v>
       </c>
-      <c r="B369" s="1" t="s">
+      <c r="B369" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="1" t="n">
+      <c r="A370" s="2" t="n">
         <v>4702113</v>
       </c>
-      <c r="B370" s="1" t="s">
+      <c r="B370" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="1" t="n">
+      <c r="A371" s="2" t="n">
         <v>4702121</v>
       </c>
-      <c r="B371" s="1" t="s">
+      <c r="B371" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="1" t="n">
+      <c r="A372" s="2" t="n">
         <v>4702122</v>
       </c>
-      <c r="B372" s="1" t="s">
+      <c r="B372" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="1" t="n">
+      <c r="A373" s="2" t="n">
         <v>4702123</v>
       </c>
-      <c r="B373" s="1" t="s">
+      <c r="B373" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="1" t="n">
+      <c r="A374" s="2" t="n">
         <v>4703111</v>
       </c>
-      <c r="B374" s="1" t="s">
+      <c r="B374" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="1" t="n">
+      <c r="A375" s="2" t="n">
         <v>4703112</v>
       </c>
-      <c r="B375" s="1" t="s">
+      <c r="B375" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="1" t="n">
+      <c r="A376" s="2" t="n">
         <v>4703113</v>
       </c>
-      <c r="B376" s="1" t="s">
+      <c r="B376" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="1" t="n">
+      <c r="A377" s="2" t="n">
         <v>4703121</v>
       </c>
-      <c r="B377" s="1" t="s">
+      <c r="B377" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="1" t="n">
+      <c r="A378" s="2" t="n">
         <v>4703122</v>
       </c>
-      <c r="B378" s="1" t="s">
+      <c r="B378" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="1" t="n">
+      <c r="A379" s="2" t="n">
         <v>4703123</v>
       </c>
-      <c r="B379" s="1" t="s">
+      <c r="B379" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="1" t="n">
+      <c r="A380" s="2" t="n">
         <v>4704111</v>
       </c>
-      <c r="B380" s="1" t="s">
+      <c r="B380" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="1" t="n">
+      <c r="A381" s="2" t="n">
         <v>4704112</v>
       </c>
-      <c r="B381" s="1" t="s">
+      <c r="B381" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="1" t="n">
+      <c r="A382" s="2" t="n">
         <v>4704113</v>
       </c>
-      <c r="B382" s="1" t="s">
+      <c r="B382" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="1" t="n">
+      <c r="A383" s="2" t="n">
         <v>4704121</v>
       </c>
-      <c r="B383" s="1" t="s">
+      <c r="B383" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="1" t="n">
+      <c r="A384" s="2" t="n">
         <v>4704122</v>
       </c>
-      <c r="B384" s="1" t="s">
+      <c r="B384" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="1" t="n">
+      <c r="A385" s="2" t="n">
         <v>4704123</v>
       </c>
-      <c r="B385" s="1" t="s">
+      <c r="B385" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="1" t="n">
+      <c r="A386" s="2" t="n">
         <v>4705111</v>
       </c>
-      <c r="B386" s="1" t="s">
+      <c r="B386" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="1" t="n">
+      <c r="A387" s="2" t="n">
         <v>4705112</v>
       </c>
-      <c r="B387" s="1" t="s">
+      <c r="B387" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="1" t="n">
+      <c r="A388" s="2" t="n">
         <v>4705113</v>
       </c>
-      <c r="B388" s="1" t="s">
+      <c r="B388" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="1" t="n">
+      <c r="A389" s="2" t="n">
         <v>4705121</v>
       </c>
-      <c r="B389" s="1" t="s">
+      <c r="B389" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="1" t="n">
+      <c r="A390" s="2" t="n">
         <v>4705122</v>
       </c>
-      <c r="B390" s="1" t="s">
+      <c r="B390" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="1" t="n">
+      <c r="A391" s="2" t="n">
         <v>4705123</v>
       </c>
-      <c r="B391" s="1" t="s">
+      <c r="B391" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="1" t="n">
+      <c r="A392" s="2" t="n">
         <v>4706111</v>
       </c>
-      <c r="B392" s="1" t="s">
+      <c r="B392" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="1" t="n">
+      <c r="A393" s="2" t="n">
         <v>4706112</v>
       </c>
-      <c r="B393" s="1" t="s">
+      <c r="B393" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="1" t="n">
+      <c r="A394" s="2" t="n">
         <v>4706113</v>
       </c>
-      <c r="B394" s="1" t="s">
+      <c r="B394" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="1" t="n">
+      <c r="A395" s="2" t="n">
         <v>4706121</v>
       </c>
-      <c r="B395" s="1" t="s">
+      <c r="B395" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="1" t="n">
+      <c r="A396" s="2" t="n">
         <v>4706122</v>
       </c>
-      <c r="B396" s="1" t="s">
+      <c r="B396" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="1" t="n">
+      <c r="A397" s="2" t="n">
         <v>4706123</v>
       </c>
-      <c r="B397" s="1" t="s">
+      <c r="B397" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="1" t="n">
+      <c r="A398" s="2" t="n">
         <v>4707111</v>
       </c>
-      <c r="B398" s="1" t="s">
+      <c r="B398" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="1" t="n">
+      <c r="A399" s="2" t="n">
         <v>4707112</v>
       </c>
-      <c r="B399" s="1" t="s">
+      <c r="B399" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="1" t="n">
+      <c r="A400" s="2" t="n">
         <v>4707113</v>
       </c>
-      <c r="B400" s="1" t="s">
+      <c r="B400" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="1" t="n">
+      <c r="A401" s="2" t="n">
         <v>4707121</v>
       </c>
-      <c r="B401" s="1" t="s">
+      <c r="B401" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="1" t="n">
+      <c r="A402" s="2" t="n">
         <v>4707122</v>
       </c>
-      <c r="B402" s="1" t="s">
+      <c r="B402" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="1" t="n">
+      <c r="A403" s="2" t="n">
         <v>4707123</v>
       </c>
-      <c r="B403" s="1" t="s">
+      <c r="B403" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="1" t="n">
+      <c r="A404" s="2" t="n">
         <v>4708111</v>
       </c>
-      <c r="B404" s="1" t="s">
+      <c r="B404" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="1" t="n">
+      <c r="A405" s="2" t="n">
         <v>4708112</v>
       </c>
-      <c r="B405" s="1" t="s">
+      <c r="B405" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="1" t="n">
+      <c r="A406" s="2" t="n">
         <v>4708113</v>
       </c>
-      <c r="B406" s="1" t="s">
+      <c r="B406" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="1" t="n">
+      <c r="A407" s="2" t="n">
         <v>4708121</v>
       </c>
-      <c r="B407" s="1" t="s">
+      <c r="B407" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="1" t="n">
+      <c r="A408" s="2" t="n">
         <v>4708122</v>
       </c>
-      <c r="B408" s="1" t="s">
+      <c r="B408" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="1" t="n">
+      <c r="A409" s="2" t="n">
         <v>4708123</v>
       </c>
-      <c r="B409" s="1" t="s">
+      <c r="B409" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="1" t="n">
+      <c r="A410" s="2" t="n">
         <v>4709111</v>
       </c>
-      <c r="B410" s="1" t="s">
+      <c r="B410" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="1" t="n">
+      <c r="A411" s="2" t="n">
         <v>4709112</v>
       </c>
-      <c r="B411" s="1" t="s">
+      <c r="B411" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="1" t="n">
+      <c r="A412" s="2" t="n">
         <v>4709113</v>
       </c>
-      <c r="B412" s="1" t="s">
+      <c r="B412" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="1" t="n">
+      <c r="A413" s="2" t="n">
         <v>4709121</v>
       </c>
-      <c r="B413" s="1" t="s">
+      <c r="B413" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="1" t="n">
+      <c r="A414" s="2" t="n">
         <v>4709122</v>
       </c>
-      <c r="B414" s="1" t="s">
+      <c r="B414" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="1" t="n">
+      <c r="A415" s="2" t="n">
         <v>4709123</v>
       </c>
-      <c r="B415" s="1" t="s">
+      <c r="B415" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="1" t="n">
+      <c r="A416" s="2" t="n">
         <v>4710111</v>
       </c>
-      <c r="B416" s="1" t="s">
+      <c r="B416" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="1" t="n">
+      <c r="A417" s="2" t="n">
         <v>4710112</v>
       </c>
-      <c r="B417" s="1" t="s">
+      <c r="B417" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="1" t="n">
+      <c r="A418" s="2" t="n">
         <v>4710113</v>
       </c>
-      <c r="B418" s="1" t="s">
+      <c r="B418" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="1" t="n">
+      <c r="A419" s="2" t="n">
         <v>4710121</v>
       </c>
-      <c r="B419" s="1" t="s">
+      <c r="B419" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="1" t="n">
+      <c r="A420" s="2" t="n">
         <v>4710122</v>
       </c>
-      <c r="B420" s="1" t="s">
+      <c r="B420" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="1" t="n">
+      <c r="A421" s="2" t="n">
         <v>4710123</v>
       </c>
-      <c r="B421" s="1" t="s">
+      <c r="B421" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>